<commit_message>
Load parameters from dataframe for Epilepsy
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Epilepsy.xlsx
+++ b/resources/ResourceFile_Epilepsy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Phillips\PycharmProjects\TLOmodel\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93879E60-0BE6-C148-919B-CA3E12359E30}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="2620" windowWidth="22920" windowHeight="13680" activeTab="2"/>
+    <workbookView xWindow="14760" yWindow="-22580" windowWidth="19200" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="108">
   <si>
     <t>Name:</t>
   </si>
@@ -337,25 +338,28 @@
     <t>rr_stop_antiepileptic_seiz_infreq_or_freq</t>
   </si>
   <si>
-    <t>value2</t>
-  </si>
-  <si>
-    <t>value3</t>
-  </si>
-  <si>
-    <t>value4</t>
-  </si>
-  <si>
     <t>relative rate of stopping antiepileptics if having infrequent or frequent seizures</t>
   </si>
   <si>
     <t>0.9875, 0.004, 0.008, 0.0005</t>
+  </si>
+  <si>
+    <t>[0.9875, 0.004, 0.008, 0.0005]</t>
+  </si>
+  <si>
+    <t>daly_wt_epilepsy_severe</t>
+  </si>
+  <si>
+    <t>daly_wt_epilepsy_less_severe</t>
+  </si>
+  <si>
+    <t>daly_wt_epilepsy_seizure_free</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -650,7 +654,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5062AFF-693C-6A42-A173-3AAA30FCCCE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -741,7 +745,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="293" name="Picture 292"/>
+        <xdr:cNvPr id="293" name="Picture 292">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000025010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -779,7 +789,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -817,7 +833,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -860,7 +882,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -915,7 +943,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -970,7 +1004,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1025,7 +1065,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1080,7 +1126,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1135,7 +1187,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1474,20 +1532,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="90.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1495,10 +1553,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1506,19 +1564,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
@@ -1526,10 +1584,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
@@ -1537,10 +1595,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="2:3" ht="95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>4</v>
       </c>
@@ -1548,7 +1606,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>25</v>
       </c>
@@ -1556,37 +1614,37 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
@@ -1594,13 +1652,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -1608,7 +1666,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -1616,13 +1674,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>10</v>
       </c>
@@ -1630,7 +1688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1696,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>8</v>
       </c>
@@ -1650,27 +1708,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A30:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A30" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.08203125" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="42.1640625" customWidth="1"/>
-    <col min="4" max="4" width="102.75" customWidth="1"/>
-    <col min="5" max="5" width="180.25" customWidth="1"/>
+    <col min="4" max="4" width="102.6640625" customWidth="1"/>
+    <col min="5" max="5" width="180.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>20</v>
       </c>
@@ -1681,7 +1739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>36</v>
       </c>
@@ -1690,7 +1748,7 @@
       </c>
       <c r="E33" s="14"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>37</v>
       </c>
@@ -1698,7 +1756,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>38</v>
       </c>
@@ -1707,7 +1765,7 @@
       </c>
       <c r="E35" s="14"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>16</v>
       </c>
@@ -1721,12 +1779,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D40" t="s">
         <v>46</v>
@@ -1735,7 +1793,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>42</v>
       </c>
@@ -1749,7 +1807,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>44</v>
       </c>
@@ -1763,7 +1821,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="25" t="s">
         <v>48</v>
       </c>
@@ -1777,7 +1835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>51</v>
       </c>
@@ -1791,7 +1849,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>53</v>
       </c>
@@ -1805,7 +1863,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="28" t="s">
         <v>67</v>
       </c>
@@ -1819,7 +1877,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>53</v>
       </c>
@@ -1833,7 +1891,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>55</v>
       </c>
@@ -1847,7 +1905,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="25" t="s">
         <v>57</v>
       </c>
@@ -1861,7 +1919,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="25" t="s">
         <v>76</v>
       </c>
@@ -1875,7 +1933,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="25" t="s">
         <v>60</v>
       </c>
@@ -1889,7 +1947,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="25" t="s">
         <v>61</v>
       </c>
@@ -1903,7 +1961,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="27" t="s">
         <v>91</v>
       </c>
@@ -1917,7 +1975,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="27" t="s">
         <v>64</v>
       </c>
@@ -1931,7 +1989,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>101</v>
       </c>
@@ -1939,11 +1997,11 @@
         <v>0.5</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E55" s="29"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="25" t="s">
         <v>92</v>
       </c>
@@ -1957,21 +2015,21 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E57" s="15"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E58" s="29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="25"/>
       <c r="D59" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>79</v>
       </c>
@@ -1979,17 +2037,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>71</v>
       </c>
@@ -1997,34 +2055,34 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="17"/>
       <c r="D68" s="17"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
       <c r="D69" s="17"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
       <c r="D70" s="17"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
       <c r="D71" s="17"/>
     </row>
@@ -2036,62 +2094,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.83203125" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="23.25" customWidth="1"/>
-    <col min="5" max="5" width="13.9140625" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2">
-        <v>0.98750000000000004</v>
-      </c>
-      <c r="C2">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D2">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="E2">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -2099,7 +2142,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -2108,7 +2151,7 @@
       </c>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2117,7 +2160,7 @@
       </c>
       <c r="I5" s="16"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2126,7 +2169,7 @@
       </c>
       <c r="I6" s="16"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -2135,7 +2178,7 @@
       </c>
       <c r="I7" s="16"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -2143,7 +2186,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -2151,7 +2194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2159,7 +2202,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -2167,7 +2210,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -2175,7 +2218,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2183,7 +2226,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2194,7 +2237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2202,7 +2245,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -2210,7 +2253,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -2221,7 +2264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -2229,51 +2272,76 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>92</v>
       </c>
       <c r="B19">
-        <v>1E-3</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:E598"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="592" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B592" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="594" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B594" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="596" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B596" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="598" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B598" t="s">
         <v>19</v>
       </c>

</xml_diff>